<commit_message>
Fixed constant variable column. Highlighted the changed made to weight column. Patrice to check rest of weighted columm, models used to clear up where possible and pub bias
</commit_message>
<xml_diff>
--- a/data/MA_CompPysio_Survey_original.xlsx
+++ b/data/MA_CompPysio_Survey_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielnoble/Dropbox/1_Research/1_Manuscripts/In_Preparation/Effects_ComparativePhysiology_Meta-analysis_Specialssue/meta_physiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4B72BCD0-197A-7E45-8B4A-E0FB02A5C8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{33171894-075D-914A-A568-DD8A16A3CD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68800" yWindow="-5400" windowWidth="25040" windowHeight="14500"/>
+    <workbookView xWindow="71920" yWindow="-5480" windowWidth="25040" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="MA_CompPysio_Survey_original" sheetId="1" r:id="rId1"/>
@@ -3505,17 +3505,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="R51" sqref="R48:R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="11" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="52.1640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="52.1640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
     <col min="14" max="14" width="43.1640625" customWidth="1"/>
+    <col min="16" max="16" width="27" customWidth="1"/>
+    <col min="18" max="18" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.2">
@@ -4072,7 +4073,7 @@
       <c r="Q6" t="s">
         <v>124</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S6" t="s">
@@ -4185,7 +4186,7 @@
       <c r="Q7" t="s">
         <v>145</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S7" t="s">
@@ -4387,7 +4388,7 @@
       <c r="Q9" t="s">
         <v>182</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S9" t="s">
@@ -5085,7 +5086,7 @@
       <c r="Q16" t="s">
         <v>275</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S16" t="s">
@@ -5810,7 +5811,7 @@
       <c r="M23" t="s">
         <v>390</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O23" t="s">
@@ -5908,7 +5909,7 @@
       <c r="M24" t="s">
         <v>405</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O24" t="s">
@@ -6006,7 +6007,7 @@
       <c r="M25" t="s">
         <v>418</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O25" t="s">
@@ -6116,7 +6117,7 @@
       <c r="M26" t="s">
         <v>432</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O26" t="s">
@@ -6205,7 +6206,7 @@
       <c r="M27" t="s">
         <v>442</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O27" t="s">
@@ -6306,7 +6307,7 @@
       <c r="M28" t="s">
         <v>454</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O28" t="s">
@@ -6407,7 +6408,7 @@
       <c r="M29" t="s">
         <v>467</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P29" t="s">
@@ -6499,7 +6500,7 @@
       <c r="M30" t="s">
         <v>479</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P30" t="s">
@@ -6508,7 +6509,7 @@
       <c r="Q30" t="s">
         <v>480</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30" s="3" t="s">
         <v>88</v>
       </c>
       <c r="S30" t="s">
@@ -6600,7 +6601,7 @@
       <c r="M31" t="s">
         <v>493</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="3" t="s">
         <v>57</v>
       </c>
       <c r="O31" t="s">
@@ -6704,7 +6705,7 @@
       <c r="M32" t="s">
         <v>509</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O32" t="s">
@@ -6799,7 +6800,7 @@
       <c r="M33" t="s">
         <v>521</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O33" t="s">
@@ -6900,7 +6901,7 @@
       <c r="M34" t="s">
         <v>534</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O34" t="s">
@@ -7004,7 +7005,7 @@
       <c r="M35" t="s">
         <v>548</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="3" t="s">
         <v>57</v>
       </c>
       <c r="O35" t="s">
@@ -7105,7 +7106,7 @@
       <c r="M36" t="s">
         <v>257</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O36" t="s">
@@ -7206,7 +7207,7 @@
       <c r="M37" t="s">
         <v>257</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O37" t="s">
@@ -7301,7 +7302,7 @@
       <c r="M38" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="3" t="s">
         <v>45</v>
       </c>
       <c r="O38" t="s">
@@ -7402,7 +7403,7 @@
       <c r="M39" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O39" t="s">
@@ -7500,7 +7501,7 @@
       <c r="M40" t="s">
         <v>611</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P40" t="s">
@@ -7583,7 +7584,7 @@
       <c r="M41" t="s">
         <v>625</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O41" t="s">
@@ -7678,7 +7679,7 @@
       <c r="M42" t="s">
         <v>639</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P42" t="s">
@@ -7779,7 +7780,7 @@
       <c r="M43" t="s">
         <v>625</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O43" t="s">
@@ -7880,7 +7881,7 @@
       <c r="M44" t="s">
         <v>664</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P44" t="s">
@@ -7981,7 +7982,7 @@
       <c r="M45" t="s">
         <v>677</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P45" t="s">
@@ -8070,13 +8071,13 @@
       <c r="K46" t="s">
         <v>687</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="L46" s="3" t="s">
         <v>688</v>
       </c>
       <c r="M46" t="s">
         <v>689</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P46" t="s">
@@ -8165,7 +8166,7 @@
       <c r="M47" t="s">
         <v>700</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P47" t="s">
@@ -8257,7 +8258,7 @@
       <c r="M48" t="s">
         <v>709</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N48" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P48" t="s">
@@ -8343,7 +8344,7 @@
       <c r="M49" t="s">
         <v>700</v>
       </c>
-      <c r="N49" t="s">
+      <c r="N49" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P49" t="s">
@@ -8441,7 +8442,7 @@
       <c r="M50" t="s">
         <v>730</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P50" t="s">
@@ -8524,7 +8525,7 @@
       <c r="M51" t="s">
         <v>739</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N51" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P51" t="s">
@@ -8604,7 +8605,7 @@
       <c r="M52" t="s">
         <v>746</v>
       </c>
-      <c r="N52" t="s">
+      <c r="N52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P52" t="s">
@@ -8705,7 +8706,7 @@
       <c r="M53" t="s">
         <v>758</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O53" t="s">
@@ -8809,7 +8810,7 @@
       <c r="M54" t="s">
         <v>772</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P54" t="s">
@@ -8904,7 +8905,7 @@
       <c r="M55" t="s">
         <v>785</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N55" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O55" t="s">
@@ -9011,7 +9012,7 @@
       <c r="M56" t="s">
         <v>798</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N56" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P56" t="s">
@@ -9109,7 +9110,7 @@
       <c r="M57" t="s">
         <v>809</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N57" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P57" t="s">
@@ -9210,7 +9211,7 @@
       <c r="M58" t="s">
         <v>820</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P58" t="s">
@@ -9311,7 +9312,7 @@
       <c r="M59" t="s">
         <v>828</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N59" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O59" t="s">
@@ -9406,7 +9407,7 @@
       <c r="M60" t="s">
         <v>838</v>
       </c>
-      <c r="N60" t="s">
+      <c r="N60" s="3" t="s">
         <v>57</v>
       </c>
       <c r="O60" s="1" t="s">
@@ -9504,7 +9505,7 @@
       <c r="M61" t="s">
         <v>847</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P61" t="s">
@@ -9608,7 +9609,7 @@
       <c r="M62" t="s">
         <v>858</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" s="3" t="s">
         <v>57</v>
       </c>
       <c r="P62" t="s">
@@ -9706,7 +9707,7 @@
       <c r="M63" t="s">
         <v>625</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N63" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O63" t="s">

</xml_diff>

<commit_message>
Corrected mistake survey data
</commit_message>
<xml_diff>
--- a/data/MA_CompPysio_Survey_original.xlsx
+++ b/data/MA_CompPysio_Survey_original.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5288536_ad_unsw_edu_au/Documents/[ PhD UNSW ]/Side project - Meta-analysis in comparative physiology/meta_physiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="13_ncr:40009_{33171894-075D-914A-A568-DD8A16A3CD76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1BB2339-9AF3-4E2E-A498-FC3D1BFD8C3D}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="13_ncr:40009_{33171894-075D-914A-A568-DD8A16A3CD76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A268921-58A2-429D-A14A-F2AE2EC9065B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3511,8 +3511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO13" sqref="AO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4761,10 +4761,10 @@
       <c r="AI10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AJ10" s="1" t="s">
+      <c r="AJ10" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="AK10" s="1" t="s">
+      <c r="AK10" s="4" t="s">
         <v>174</v>
       </c>
       <c r="AL10" s="1"/>

</xml_diff>

<commit_message>
Following reviewer's recommendation - data extraction of one additional study
</commit_message>
<xml_diff>
--- a/data/MA_CompPysio_Survey_original.xlsx
+++ b/data/MA_CompPysio_Survey_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielnoble/Dropbox/1_Research/1_Manuscripts/In_Preparation/Effects_ComparativePhysiology_Meta-analysis_Specialssue/meta_physiology/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5288536_ad_unsw_edu_au/Documents/[ PhD UNSW ]/Side project - Meta-analysis in comparative physiology/meta_physiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40257B35-2827-3842-8931-71E08B1A35E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{40257B35-2827-3842-8931-71E08B1A35E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E144AE07-30C7-40A6-913B-657EFEFBDCC9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_CompPysio_Survey_original" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="875">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2645,6 +2645,24 @@
   </si>
   <si>
     <t>Dryad (https://datadryad.org/stash/dataset/doi:10.5061/dryad.6rn80)</t>
+  </si>
+  <si>
+    <t>Costs of immune responses are related to host body size and lifespan</t>
+  </si>
+  <si>
+    <t>Brace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They compared the responses of control groups and treatment groups treated with an immune system stimulant. However, they did not control for dose-dependent effects. </t>
+  </si>
+  <si>
+    <t>They performed analyses with, and without phylogeny.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They accounted for shared control groups by modelling the covariance between the dependent effect sizes, and included a species-level random effect and phylogenetic relatedness. </t>
+  </si>
+  <si>
+    <t>SI (https://onlinelibrary.wiley.com/action/downloadSupplement?doi=10.1002%2Fjez.2084&amp;file=jez2084-sup-0001-SuppMat.pdf)</t>
   </si>
 </sst>
 </file>
@@ -3146,7 +3164,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -3154,6 +3172,8 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3511,23 +3531,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO69" sqref="AO69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="11" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="28.6640625" customWidth="1"/>
+    <col min="3" max="5" width="10.875" customWidth="1"/>
+    <col min="6" max="11" width="10.875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="28.625" customWidth="1"/>
     <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="43.1640625" customWidth="1"/>
+    <col min="14" max="14" width="43.125" customWidth="1"/>
     <col min="16" max="16" width="27" customWidth="1"/>
-    <col min="18" max="18" width="42.6640625" customWidth="1"/>
+    <col min="18" max="18" width="42.625" customWidth="1"/>
     <col min="36" max="36" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3665,7 +3686,7 @@
       <c r="BF1" s="1"/>
       <c r="BG1" s="1"/>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -3783,7 +3804,7 @@
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -3899,7 +3920,7 @@
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>77</v>
       </c>
@@ -4031,7 +4052,7 @@
       <c r="BF4" s="1"/>
       <c r="BG4" s="1"/>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -4155,7 +4176,7 @@
       <c r="BF5" s="1"/>
       <c r="BG5" s="1"/>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -4289,7 +4310,7 @@
       <c r="BF6" s="1"/>
       <c r="BG6" s="1"/>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>135</v>
       </c>
@@ -4423,7 +4444,7 @@
       <c r="BF7" s="1"/>
       <c r="BG7" s="1"/>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>158</v>
       </c>
@@ -4545,7 +4566,7 @@
       <c r="BF8" s="1"/>
       <c r="BG8" s="1"/>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>175</v>
       </c>
@@ -4673,7 +4694,7 @@
       <c r="BF9" s="1"/>
       <c r="BG9" s="1"/>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>189</v>
       </c>
@@ -4793,7 +4814,7 @@
       <c r="BF10" s="1"/>
       <c r="BG10" s="1"/>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>201</v>
       </c>
@@ -4917,7 +4938,7 @@
       <c r="BF11" s="1"/>
       <c r="BG11" s="1"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>214</v>
       </c>
@@ -5043,7 +5064,7 @@
       <c r="BF12" s="1"/>
       <c r="BG12" s="1"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>228</v>
       </c>
@@ -5169,7 +5190,7 @@
       <c r="BF13" s="1"/>
       <c r="BG13" s="1"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>241</v>
       </c>
@@ -5293,7 +5314,7 @@
       <c r="BF14" s="1"/>
       <c r="BG14" s="1"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>252</v>
       </c>
@@ -5419,7 +5440,7 @@
       <c r="BF15" s="1"/>
       <c r="BG15" s="1"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>266</v>
       </c>
@@ -5553,7 +5574,7 @@
       <c r="BF16" s="1"/>
       <c r="BG16" s="1"/>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>288</v>
       </c>
@@ -5679,7 +5700,7 @@
       <c r="BF17" s="1"/>
       <c r="BG17" s="1"/>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>300</v>
       </c>
@@ -5807,7 +5828,7 @@
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>320</v>
       </c>
@@ -5933,7 +5954,7 @@
       <c r="BF19" s="1"/>
       <c r="BG19" s="1"/>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>335</v>
       </c>
@@ -6065,7 +6086,7 @@
       <c r="BF20" s="1"/>
       <c r="BG20" s="1"/>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>354</v>
       </c>
@@ -6197,7 +6218,7 @@
       <c r="BF21" s="1"/>
       <c r="BG21" s="1"/>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>372</v>
       </c>
@@ -6321,7 +6342,7 @@
       <c r="BF22" s="1"/>
       <c r="BG22" s="1"/>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>385</v>
       </c>
@@ -6447,7 +6468,7 @@
       <c r="BF23" s="1"/>
       <c r="BG23" s="1"/>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>400</v>
       </c>
@@ -6569,7 +6590,7 @@
       <c r="BF24" s="1"/>
       <c r="BG24" s="1"/>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>413</v>
       </c>
@@ -6701,7 +6722,7 @@
       <c r="BF25" s="1"/>
       <c r="BG25" s="1"/>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>427</v>
       </c>
@@ -6821,7 +6842,7 @@
       <c r="BF26" s="1"/>
       <c r="BG26" s="1"/>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>438</v>
       </c>
@@ -6945,7 +6966,7 @@
       <c r="BF27" s="1"/>
       <c r="BG27" s="1"/>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>449</v>
       </c>
@@ -7071,7 +7092,7 @@
       <c r="BF28" s="1"/>
       <c r="BG28" s="1"/>
     </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>461</v>
       </c>
@@ -7189,7 +7210,7 @@
       <c r="BF29" s="1"/>
       <c r="BG29" s="1"/>
     </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>473</v>
       </c>
@@ -7317,7 +7338,7 @@
       <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>488</v>
       </c>
@@ -7445,7 +7466,7 @@
       <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
     </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>504</v>
       </c>
@@ -7567,7 +7588,7 @@
       <c r="BF32" s="1"/>
       <c r="BG32" s="1"/>
     </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>515</v>
       </c>
@@ -7693,7 +7714,7 @@
       <c r="BF33" s="1"/>
       <c r="BG33" s="1"/>
     </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>529</v>
       </c>
@@ -7821,7 +7842,7 @@
       <c r="BF34" s="1"/>
       <c r="BG34" s="1"/>
     </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>543</v>
       </c>
@@ -7947,7 +7968,7 @@
       <c r="BF35" s="1"/>
       <c r="BG35" s="1"/>
     </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>556</v>
       </c>
@@ -8073,7 +8094,7 @@
       <c r="BF36" s="1"/>
       <c r="BG36" s="1"/>
     </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>567</v>
       </c>
@@ -8195,7 +8216,7 @@
       <c r="BF37" s="1"/>
       <c r="BG37" s="1"/>
     </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>578</v>
       </c>
@@ -8321,7 +8342,7 @@
       <c r="BF38" s="1"/>
       <c r="BG38" s="1"/>
     </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>592</v>
       </c>
@@ -8445,7 +8466,7 @@
       <c r="BF39" s="1"/>
       <c r="BG39" s="1"/>
     </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>606</v>
       </c>
@@ -8561,7 +8582,7 @@
       <c r="BF40" s="1"/>
       <c r="BG40" s="1"/>
     </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>620</v>
       </c>
@@ -8683,7 +8704,7 @@
       <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
     </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>635</v>
       </c>
@@ -8807,7 +8828,7 @@
       <c r="BF42" s="1"/>
       <c r="BG42" s="1"/>
     </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>648</v>
       </c>
@@ -8933,7 +8954,7 @@
       <c r="BF43" s="1"/>
       <c r="BG43" s="1"/>
     </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>659</v>
       </c>
@@ -9059,7 +9080,7 @@
       <c r="BF44" s="1"/>
       <c r="BG44" s="1"/>
     </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>673</v>
       </c>
@@ -9183,7 +9204,7 @@
       <c r="BF45" s="1"/>
       <c r="BG45" s="1"/>
     </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>684</v>
       </c>
@@ -9301,7 +9322,7 @@
       <c r="BF46" s="1"/>
       <c r="BG46" s="1"/>
     </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>697</v>
       </c>
@@ -9421,7 +9442,7 @@
       <c r="BF47" s="1"/>
       <c r="BG47" s="1"/>
     </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>705</v>
       </c>
@@ -9535,7 +9556,7 @@
       <c r="BF48" s="1"/>
       <c r="BG48" s="1"/>
     </row>
-    <row r="49" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>712</v>
       </c>
@@ -9661,7 +9682,7 @@
       <c r="BF49" s="1"/>
       <c r="BG49" s="1"/>
     </row>
-    <row r="50" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>726</v>
       </c>
@@ -9775,7 +9796,7 @@
       <c r="BF50" s="1"/>
       <c r="BG50" s="1"/>
     </row>
-    <row r="51" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>735</v>
       </c>
@@ -9887,7 +9908,7 @@
       <c r="BF51" s="1"/>
       <c r="BG51" s="1"/>
     </row>
-    <row r="52" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>742</v>
       </c>
@@ -10011,7 +10032,7 @@
       <c r="BF52" s="1"/>
       <c r="BG52" s="1"/>
     </row>
-    <row r="53" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>753</v>
       </c>
@@ -10139,7 +10160,7 @@
       <c r="BF53" s="1"/>
       <c r="BG53" s="1"/>
     </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>767</v>
       </c>
@@ -10261,7 +10282,7 @@
       <c r="BF54" s="1"/>
       <c r="BG54" s="1"/>
     </row>
-    <row r="55" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>780</v>
       </c>
@@ -10391,7 +10412,7 @@
       <c r="BF55" s="1"/>
       <c r="BG55" s="1"/>
     </row>
-    <row r="56" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>793</v>
       </c>
@@ -10515,7 +10536,7 @@
       <c r="BF56" s="1"/>
       <c r="BG56" s="1"/>
     </row>
-    <row r="57" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>804</v>
       </c>
@@ -10641,7 +10662,7 @@
       <c r="BF57" s="1"/>
       <c r="BG57" s="1"/>
     </row>
-    <row r="58" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>815</v>
       </c>
@@ -10767,7 +10788,7 @@
       <c r="BF58" s="1"/>
       <c r="BG58" s="1"/>
     </row>
-    <row r="59" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>824</v>
       </c>
@@ -10889,7 +10910,7 @@
       <c r="BF59" s="1"/>
       <c r="BG59" s="1"/>
     </row>
-    <row r="60" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>834</v>
       </c>
@@ -11013,7 +11034,7 @@
       <c r="BF60" s="1"/>
       <c r="BG60" s="1"/>
     </row>
-    <row r="61" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>843</v>
       </c>
@@ -11141,7 +11162,7 @@
       <c r="BF61" s="1"/>
       <c r="BG61" s="1"/>
     </row>
-    <row r="62" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>854</v>
       </c>
@@ -11267,7 +11288,7 @@
       <c r="BF62" s="1"/>
       <c r="BG62" s="1"/>
     </row>
-    <row r="63" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>862</v>
       </c>
@@ -11387,67 +11408,123 @@
       <c r="BF63" s="1"/>
       <c r="BG63" s="1"/>
     </row>
-    <row r="64" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="1"/>
-      <c r="AA64" s="1"/>
-      <c r="AB64" s="1"/>
-      <c r="AC64" s="1"/>
-      <c r="AD64" s="1"/>
-      <c r="AE64" s="1"/>
-      <c r="AF64" s="1"/>
-      <c r="AG64" s="1"/>
-      <c r="AH64" s="1"/>
-      <c r="AI64" s="1"/>
-      <c r="AJ64" s="1"/>
-      <c r="AK64" s="1"/>
-      <c r="AL64" s="1"/>
-      <c r="AM64" s="1"/>
-      <c r="AN64" s="1"/>
-      <c r="AO64" s="1"/>
-      <c r="AP64" s="1"/>
-      <c r="AQ64" s="1"/>
-      <c r="AR64" s="1"/>
-      <c r="AS64" s="1"/>
-      <c r="AT64" s="1"/>
-      <c r="AU64" s="1"/>
-      <c r="AV64" s="1"/>
-      <c r="AW64" s="1"/>
-      <c r="AX64" s="1"/>
-      <c r="AY64" s="1"/>
-      <c r="AZ64" s="1"/>
-      <c r="BA64" s="1"/>
-      <c r="BB64" s="1"/>
-      <c r="BC64" s="1"/>
-      <c r="BD64" s="1"/>
-      <c r="BE64" s="1"/>
-      <c r="BF64" s="1"/>
-      <c r="BG64" s="1"/>
+    <row r="64" spans="1:59" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>44454</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>869</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="E64" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U64" s="6" t="s">
+        <v>873</v>
+      </c>
+      <c r="V64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W64" s="6"/>
+      <c r="Y64" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z64" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="AA64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB64" s="6"/>
+      <c r="AC64" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD64" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="AE64" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF64" s="6"/>
+      <c r="AG64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH64" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ64" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK64" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL64" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM64" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN64" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AO64" s="6"/>
+      <c r="AP64" s="6"/>
+      <c r="AQ64" s="6"/>
+      <c r="AR64" s="6"/>
+      <c r="AS64" s="6"/>
+      <c r="AT64" s="6"/>
+      <c r="AU64" s="6"/>
+      <c r="AV64" s="6"/>
+      <c r="AW64" s="6"/>
+      <c r="AX64" s="6"/>
+      <c r="AY64" s="6"/>
+      <c r="AZ64" s="6"/>
+      <c r="BA64" s="6"/>
+      <c r="BB64" s="6"/>
+      <c r="BC64" s="6"/>
+      <c r="BD64" s="6"/>
+      <c r="BE64" s="6"/>
+      <c r="BF64" s="6"/>
+      <c r="BG64" s="6"/>
     </row>
-    <row r="65" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>

</xml_diff>

<commit_message>
Updated second file + homogeneised responses to Q3.5 and Q3.6 between researchers
</commit_message>
<xml_diff>
--- a/data/MA_CompPysio_Survey_original.xlsx
+++ b/data/MA_CompPysio_Survey_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5288536_ad_unsw_edu_au/Documents/[ PhD UNSW ]/Side project - Meta-analysis in comparative physiology/meta_physiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{40257B35-2827-3842-8931-71E08B1A35E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E144AE07-30C7-40A6-913B-657EFEFBDCC9}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{40257B35-2827-3842-8931-71E08B1A35E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB425303-BF0B-4AC8-98A5-5A768AA4485D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_CompPysio_Survey_original" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="877">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2663,6 +2663,12 @@
   </si>
   <si>
     <t>SI (https://onlinelibrary.wiley.com/action/downloadSupplement?doi=10.1002%2Fjez.2084&amp;file=jez2084-sup-0001-SuppMat.pdf)</t>
+  </si>
+  <si>
+    <t>"unclear/other"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors estimated "fixed-effect Qwithin", which is described as testing for the evidence of a file drawer problem. </t>
   </si>
 </sst>
 </file>
@@ -3531,9 +3537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO69" sqref="AO69"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI66" sqref="AI66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8557,11 +8563,21 @@
       <c r="AI40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AJ40" s="1"/>
-      <c r="AK40" s="1"/>
-      <c r="AL40" s="1"/>
-      <c r="AM40" s="1"/>
-      <c r="AN40" s="1"/>
+      <c r="AJ40" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL40" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN40" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="AO40" s="1"/>
       <c r="AP40" s="1"/>
       <c r="AQ40" s="1"/>
@@ -9772,10 +9788,18 @@
       <c r="AJ50" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="AK50" s="1"/>
-      <c r="AL50" s="1"/>
-      <c r="AM50" s="1"/>
-      <c r="AN50" s="1"/>
+      <c r="AK50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL50" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN50" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="AO50" s="1"/>
       <c r="AP50" s="1"/>
       <c r="AQ50" s="1"/>
@@ -9883,11 +9907,21 @@
       <c r="AI51" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AJ51" s="1"/>
-      <c r="AK51" s="1"/>
-      <c r="AL51" s="1"/>
-      <c r="AM51" s="1"/>
-      <c r="AN51" s="1"/>
+      <c r="AJ51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK51" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM51" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN51" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="AO51" s="1"/>
       <c r="AP51" s="1"/>
       <c r="AQ51" s="1"/>
@@ -11457,9 +11491,11 @@
         <v>873</v>
       </c>
       <c r="V64" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W64" s="6"/>
+        <v>875</v>
+      </c>
+      <c r="W64" s="6" t="s">
+        <v>876</v>
+      </c>
       <c r="Y64" s="6" t="s">
         <v>44</v>
       </c>
@@ -11586,5 +11622,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>